<commit_message>
Update data file for Children in CCI with latest information
</commit_message>
<xml_diff>
--- a/input/children-in-cci/2024-09-22_Data.xlsx
+++ b/input/children-in-cci/2024-09-22_Data.xlsx
@@ -1,65 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9553f9d3bca49a69/Office/Annual Report of SCPS/Data Analysis/input/children-in-cci/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="8_{7E4BEFA9-255C-46FF-90D6-FB750158E52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14376318-E702-47E9-B356-D99F83C8D9B3}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{44FEBFC4-443D-4528-AA53-47F3C38D5C28}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="CCI_Count" sheetId="1" r:id="rId1"/>
-    <sheet name="Child_Category" sheetId="2" r:id="rId2"/>
-    <sheet name="PurviewCCI" sheetId="3" r:id="rId3"/>
-    <sheet name="FormalEdRatio" sheetId="4" r:id="rId4"/>
-    <sheet name="VocationalTraining" sheetId="5" r:id="rId5"/>
+    <sheet name="CCI_Count" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Child_Category" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="PurviewCCI" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="FormalEdRatio" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="VocationalTraining" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
-  <si>
-    <t>Children Home</t>
-  </si>
-  <si>
-    <t>Children Home CWSN</t>
-  </si>
-  <si>
-    <t>Observation Home</t>
-  </si>
-  <si>
-    <t>Special Home/ Place of Safety</t>
-  </si>
-  <si>
-    <t>Specialized Adoption Agency</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>District</t>
   </si>
   <si>
+    <t xml:space="preserve">Children Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Children Home CWSN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observation Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Shelter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special Home/ Place of Safety</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specialized Adoption Agency</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
@@ -72,7 +55,19 @@
     <t>Birbhum</t>
   </si>
   <si>
-    <t>Dakshin Dinajpur</t>
+    <t xml:space="preserve">Koch Bihar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dakshin Dinajpur</t>
+  </si>
+  <si>
+    <t>Darjiling</t>
+  </si>
+  <si>
+    <t>Hugli</t>
+  </si>
+  <si>
+    <t>Haora</t>
   </si>
   <si>
     <t>Jalpaiguri</t>
@@ -81,6 +76,9 @@
     <t>Jhargram</t>
   </si>
   <si>
+    <t>Kalimpong</t>
+  </si>
+  <si>
     <t>Kolkata</t>
   </si>
   <si>
@@ -93,46 +91,37 @@
     <t>Nadia</t>
   </si>
   <si>
-    <t>North 24 Parganas</t>
-  </si>
-  <si>
-    <t>Purba Medinipur</t>
-  </si>
-  <si>
-    <t>South 24 Parganas</t>
-  </si>
-  <si>
-    <t>Uttar Dinajpur</t>
-  </si>
-  <si>
-    <t>Koch Bihar</t>
-  </si>
-  <si>
-    <t>Darjiling</t>
-  </si>
-  <si>
-    <t>Hugli</t>
-  </si>
-  <si>
-    <t>Haora</t>
-  </si>
-  <si>
-    <t>Paschim Barddhaman</t>
-  </si>
-  <si>
-    <t>Purba Barddhaman</t>
+    <t xml:space="preserve">North 24 Parganas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paschim Barddhaman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pashchim Medinipur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purba Barddhaman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purba Medinipur</t>
   </si>
   <si>
     <t>Puruliya</t>
   </si>
   <si>
-    <t>Pashchim Medinipur</t>
-  </si>
-  <si>
-    <t>Kalimpong</t>
-  </si>
-  <si>
-    <t>Non-CWSN CNCP</t>
+    <t xml:space="preserve">South 24 Parganas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uttar Dinajpur</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. of Children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-CWSN CNCP</t>
   </si>
   <si>
     <t>CWSN</t>
@@ -141,6 +130,15 @@
     <t>CCL</t>
   </si>
   <si>
+    <t>FY</t>
+  </si>
+  <si>
+    <t>Girls</t>
+  </si>
+  <si>
+    <t>Boys</t>
+  </si>
+  <si>
     <t>2017-18</t>
   </si>
   <si>
@@ -162,40 +160,18 @@
     <t>2023-24</t>
   </si>
   <si>
-    <t>Girls</t>
-  </si>
-  <si>
-    <t>Boys</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>No. of Children</t>
-  </si>
-  <si>
-    <t>FY</t>
-  </si>
-  <si>
-    <t>Open Shelter</t>
-  </si>
-  <si>
     <t>average</t>
-  </si>
-  <si>
-    <t>2024-25 (Dec)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -209,20 +185,20 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="10" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="9" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -241,12 +217,12 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+  <mc:AlternateContent>
+    <mc:Choice Requires="c14">
       <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
@@ -261,7 +237,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -277,11 +253,16 @@
               <a:rPr lang="en-US"/>
               <a:t>Category of Children</a:t>
             </a:r>
+            <a:endParaRPr/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr>
+      <c:spPr bwMode="auto">
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
@@ -293,7 +274,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -320,8 +301,11 @@
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
+            <c:spPr bwMode="auto">
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:gradFill>
                 <a:gsLst>
                   <a:gs pos="0">
                     <a:schemeClr val="accent6">
@@ -358,17 +342,15 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-EBC6-4612-A7C2-EEC628113D60}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
+            <c:spPr bwMode="auto">
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:gradFill>
                 <a:gsLst>
                   <a:gs pos="0">
                     <a:schemeClr val="accent5">
@@ -405,17 +387,15 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-EBC6-4612-A7C2-EEC628113D60}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
+            <c:spPr bwMode="auto">
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:gradFill>
                 <a:gsLst>
                   <a:gs pos="0">
                     <a:schemeClr val="accent4">
@@ -452,14 +432,36 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-EBC6-4612-A7C2-EEC628113D60}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dLbls>
-            <c:spPr>
+            <c:leaderLines>
+              <c:spPr bwMode="auto">
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:showBubbleSize val="0"/>
+            <c:showCatName val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showPercent val="1"/>
+            <c:showSerName val="0"/>
+            <c:showVal val="0"/>
+            <c:spPr bwMode="auto">
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
               <a:noFill/>
               <a:ln>
                 <a:noFill/>
@@ -473,7 +475,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -488,30 +490,6 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:round/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -548,24 +526,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-EBC6-4612-A7C2-EEC628113D60}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:showBubbleSize val="0"/>
+          <c:showCatName val="0"/>
+          <c:showLeaderLines val="1"/>
           <c:showLegendKey val="0"/>
+          <c:showPercent val="1"/>
+          <c:showSerName val="0"/>
           <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
-      <c:spPr>
+      <c:spPr bwMode="auto">
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
@@ -575,8 +551,12 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr>
+      <c:spPr bwMode="auto">
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
@@ -588,7 +568,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -606,16 +586,16 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
+  <c:spPr bwMode="auto">
+    <a:xfrm>
+      <a:off x="0" y="0"/>
+      <a:ext cx="0" cy="0"/>
+    </a:xfrm>
+    <a:prstGeom prst="rect">
+      <a:avLst/>
+    </a:prstGeom>
     <a:solidFill>
       <a:schemeClr val="bg1"/>
     </a:solidFill>
@@ -642,7 +622,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -697,7 +677,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -709,7 +689,10 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -720,16 +703,19 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:chartArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx2"/>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:solidFill>
         <a:schemeClr val="bg1"/>
       </a:solidFill>
@@ -743,7 +729,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -755,7 +741,7 @@
         <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -767,7 +753,10 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
@@ -780,7 +769,7 @@
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
@@ -814,7 +803,10 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -834,7 +826,10 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -843,7 +838,6 @@
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -853,7 +847,10 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -872,7 +869,10 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:noFill/>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -884,7 +884,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
@@ -893,7 +893,10 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:solidFill>
         <a:schemeClr val="dk1">
           <a:lumMod val="65000"/>
@@ -917,7 +920,10 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -936,7 +942,10 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -963,7 +972,10 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -982,7 +994,10 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -1001,7 +1016,10 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -1020,7 +1038,10 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -1042,7 +1063,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:legend>
   <cs:plotArea>
     <cs:lnRef idx="0"/>
@@ -1070,7 +1091,10 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -1081,7 +1105,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:seriesAxis>
   <cs:seriesLine>
     <cs:lnRef idx="0"/>
@@ -1090,7 +1114,10 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -1112,7 +1139,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+    <cs:defRPr sz="1600" b="1"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1123,7 +1150,10 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1141,7 +1171,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -1150,7 +1180,10 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
@@ -1174,7 +1207,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -1184,12 +1217,13 @@
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:wall>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
 </cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
+  <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>466724</xdr:colOff>
@@ -1202,17 +1236,11 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F60FC809-876A-4282-9B09-CA0C65D29E1C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="Chart 1"/>
         <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
+          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1230,8 +1258,291 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1273,108 +1584,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Aptos Display"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Aptos Narrow"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1382,7 +1599,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1408,7 +1625,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1460,16 +1677,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1485,7 +1714,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1517,7 +1746,7 @@
   </a:themeElements>
   <a:objectDefaults>
     <a:lnDef>
-      <a:spPr/>
+      <a:spPr bwMode="auto"/>
       <a:bodyPr/>
       <a:lstStyle/>
       <a:style>
@@ -1536,65 +1765,58 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362089EA-7575-4704-A8B7-8CFB541735D5}">
-  <dimension ref="A1:H24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H24"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="H2" activeCellId="0" sqref="H2:H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="16384" max="16384" width="9.140625" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" width="20.85546875"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" width="14.140625"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" width="20"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" width="17.42578125"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" width="9.140625"/>
+    <col bestFit="1" customWidth="1" min="6" max="6" width="27.28515625"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" width="26.42578125"/>
+    <col bestFit="1" customWidth="1" min="8" max="8" width="5.42578125"/>
+    <col bestFit="1" customWidth="1" min="9" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1618,9 +1840,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1644,9 +1866,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1670,9 +1892,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1696,9 +1918,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1722,9 +1944,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -1748,9 +1970,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -1774,9 +1996,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1800,9 +2022,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -1826,9 +2048,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1852,9 +2074,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1878,9 +2100,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -1904,9 +2126,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1930,9 +2152,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>8</v>
@@ -1956,9 +2178,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -1982,9 +2204,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>7</v>
@@ -2008,35 +2230,35 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
         <v>25</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>28</v>
       </c>
       <c r="B19">
         <v>12</v>
@@ -2060,7 +2282,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -2086,9 +2308,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -2112,9 +2334,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -2138,9 +2360,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B23">
         <v>6</v>
@@ -2164,9 +2386,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -2191,92 +2413,102 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32303193-396C-4E65-8959-967742AFC344}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" width="16.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>2528</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>1428</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>192</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C52D08-B08E-4C19-AAC1-5AC343A1B94F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>5931</v>
@@ -2288,9 +2520,9 @@
         <v>11001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>5795</v>
@@ -2302,9 +2534,9 @@
         <v>11799</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>7346</v>
@@ -2316,9 +2548,9 @@
         <v>13105</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>5221</v>
@@ -2330,9 +2562,9 @@
         <v>8836</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B6">
         <v>7138</v>
@@ -2344,9 +2576,9 @@
         <v>11711</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B7">
         <v>11131</v>
@@ -2358,9 +2590,9 @@
         <v>16475</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B8">
         <v>12958</v>
@@ -2373,179 +2605,185 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2956ED25-CB50-449F-914D-BCEBED34CFE3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1">
         <v>0.50955369980068466</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1">
         <v>0.46290806807288964</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1">
         <v>0.47065990190682927</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1">
         <v>0.47789022476016468</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1">
         <v>0.47187937096248245</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1">
         <v>0.54675583741089873</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1">
         <v>0.56826199145876555</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-    </row>
+    <row r="9"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A889A18-A100-4ACC-B73E-CB4B4DC0BDBA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" width="7.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2">
         <v>0.42307810567844872</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2">
         <v>0.42742471126864257</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2">
         <v>0.39869396131682211</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2">
         <v>0.37921372133676096</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2">
         <v>0.35419074400942852</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B7" s="2">
         <v>0.37807294431195831</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B8" s="2">
         <v>0.42059486459360856</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>